<commit_message>
Allow append to file
</commit_message>
<xml_diff>
--- a/xlsx/example.xlsx
+++ b/xlsx/example.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10311"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{D6E78FBC-C6ED-6242-AB7B-BDF69C2B6D92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="600" windowWidth="18500" windowHeight="15940"/>
+    <workbookView xWindow="10240" yWindow="600" windowWidth="18500" windowHeight="15940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -66,7 +67,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -112,9 +113,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Денежный 2" xfId="2"/>
+    <cellStyle name="Денежный 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 2" xfId="1"/>
+    <cellStyle name="Обычный 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -449,11 +450,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -519,7 +520,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -531,7 +532,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>